<commit_message>
adicionei a função flat field do Eduardo
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -453,332 +453,332 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.134421568627451</v>
+        <v>0.160625</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1173995098039216</v>
+        <v>0.1494485294117647</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3460196078431372</v>
+        <v>0.3810294117647058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.24975</v>
+        <v>0.2397009803921569</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2315637254901961</v>
+        <v>0.2279950980392157</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4581446078431373</v>
+        <v>0.4525612745098039</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.3518799019607843</v>
+        <v>0.3130073529411764</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3371225490196079</v>
+        <v>0.3116225490196078</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5572720588235295</v>
+        <v>0.519892156862745</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.4380539215686274</v>
+        <v>0.3857083333333333</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4353725490196078</v>
+        <v>0.3883897058823529</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6434975490196078</v>
+        <v>0.5952499999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.5231323529411765</v>
+        <v>0.4753504901960784</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5257965686274509</v>
+        <v>0.4857156862745098</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7351053921568628</v>
+        <v>0.6897009803921569</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.607406862745098</v>
+        <v>0.5735857843137255</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6099583333333334</v>
+        <v>0.5839509803921569</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8213700980392157</v>
+        <v>0.7953627450980392</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1480710784313725</v>
+        <v>0.2282352941176471</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3399436274509804</v>
+        <v>0.355125</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3005</v>
+        <v>0.337593137254902</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1794950980392157</v>
+        <v>0.2897794117647059</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5044607843137254</v>
+        <v>0.5289117647058824</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6967475490196079</v>
+        <v>0.7098848039215686</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.4819975490196078</v>
+        <v>0.4487622549019608</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2906372549019608</v>
+        <v>0.2956421568627451</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4872254901960785</v>
+        <v>0.488953431372549</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.5089117647058824</v>
+        <v>0.4752867647058824</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3877941176470588</v>
+        <v>0.374375</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6137156862745098</v>
+        <v>0.5948578431372549</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.4138308823529412</v>
+        <v>0.3936495098039215</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4760710784313725</v>
+        <v>0.4515661764705883</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4821519607843137</v>
+        <v>0.4726936274509804</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.2470024509803921</v>
+        <v>0.2216960784313725</v>
       </c>
       <c r="B13" t="n">
-        <v>0.357563725490196</v>
+        <v>0.3323700980392157</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7860220588235294</v>
+        <v>0.7474828431372549</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1900539215686274</v>
+        <v>0.2638578431372549</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2573333333333334</v>
+        <v>0.315093137254902</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4462769607843137</v>
+        <v>0.4995</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4090367647058823</v>
+        <v>0.4171691176470588</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2356960784313726</v>
+        <v>0.3069950980392157</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7646740196078431</v>
+        <v>0.7800637254901961</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.3913308823529412</v>
+        <v>0.40875</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1987720588235294</v>
+        <v>0.2534607843137255</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3851372549019608</v>
+        <v>0.4465171568627451</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.4551789215686275</v>
+        <v>0.4473970588235294</v>
       </c>
       <c r="B17" t="n">
-        <v>0.3586102941176471</v>
+        <v>0.3688357843137255</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4926985294117647</v>
+        <v>0.5011838235294117</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.6208799019607844</v>
+        <v>0.603406862745098</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4203578431372549</v>
+        <v>0.4089362745098039</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3029975490196078</v>
+        <v>0.3011446078431373</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1425710784313726</v>
+        <v>0.1967916666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5423651960784314</v>
+        <v>0.5552598039215686</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8300196078431372</v>
+        <v>0.8262475490196078</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2184436274509804</v>
+        <v>0.3017794117647059</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2263480392156863</v>
+        <v>0.3170490196078431</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5048039215686274</v>
+        <v>0.5701299019607844</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.3656691176470588</v>
+        <v>0.4174656862745098</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3390024509803922</v>
+        <v>0.4187279411764706</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7744779411764705</v>
+        <v>0.7986960784313725</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.3128186274509804</v>
+        <v>0.361061274509804</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2076862745098039</v>
+        <v>0.289</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4906348039215686</v>
+        <v>0.5510980392156862</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.4084779411764706</v>
+        <v>0.441468137254902</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4060098039215686</v>
+        <v>0.4523161764705882</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7056151960784314</v>
+        <v>0.7291544117647059</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.4510269607843138</v>
+        <v>0.4766838235294117</v>
       </c>
       <c r="B24" t="n">
-        <v>0.465156862745098</v>
+        <v>0.4994289215686274</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8012205882352941</v>
+        <v>0.8183063725490196</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.2377671568627451</v>
+        <v>0.2906470588235294</v>
       </c>
       <c r="B25" t="n">
-        <v>0.4404730392156863</v>
+        <v>0.4766666666666667</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8079264705882353</v>
+        <v>0.8158455882352942</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.2289019607843137</v>
+        <v>0.3066495098039216</v>
       </c>
       <c r="B26" t="n">
-        <v>0.2189411764705882</v>
+        <v>0.3141372549019608</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5286642156862744</v>
+        <v>0.5956642156862745</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.3109730392156863</v>
+        <v>0.3632450980392157</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2748921568627451</v>
+        <v>0.3806813725490196</v>
       </c>
       <c r="C27" t="n">
-        <v>0.7905098039215687</v>
+        <v>0.8270196078431372</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.3447328431372549</v>
+        <v>0.4167696078431373</v>
       </c>
       <c r="B28" t="n">
-        <v>0.3065343137254902</v>
+        <v>0.4025294117647059</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6417083333333333</v>
+        <v>0.7010024509803922</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.4106568627450981</v>
+        <v>0.4760906862745098</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3865833333333333</v>
+        <v>0.4688627450980392</v>
       </c>
       <c r="C29" t="n">
-        <v>0.724061274509804</v>
+        <v>0.7684607843137256</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.3990808823529412</v>
+        <v>0.4597598039215686</v>
       </c>
       <c r="B30" t="n">
-        <v>0.4396764705882353</v>
+        <v>0.5047377450980391</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7574044117647059</v>
+        <v>0.7937083333333333</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.3762598039215687</v>
+        <v>0.438406862745098</v>
       </c>
       <c r="B31" t="n">
-        <v>0.4740049019607843</v>
+        <v>0.5299338235294118</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7619705882352942</v>
+        <v>0.7946029411764706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>